<commit_message>
index html and population zero
</commit_message>
<xml_diff>
--- a/DB/excersises DB.xlsx
+++ b/DB/excersises DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Git projects\AI-fitness-program-generator\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B49AE0-0C65-43B6-8D9C-D6BF1DDE198B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98590279-B5AD-494A-8799-2435871A27E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="527" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,18 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="163">
   <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Equipment</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Squat</t>
   </si>
   <si>
@@ -450,15 +438,6 @@
     <t>Hammer Curl Rope</t>
   </si>
   <si>
-    <t>Is Complex</t>
-  </si>
-  <si>
-    <t>Primary Target</t>
-  </si>
-  <si>
-    <t>Secondary Target</t>
-  </si>
-  <si>
     <t>Glutes</t>
   </si>
   <si>
@@ -514,6 +493,27 @@
   </si>
   <si>
     <t>Lats, Shoulders</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>primaryTarget</t>
+  </si>
+  <si>
+    <t>secondaryTarget</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>isComplex</t>
   </si>
 </sst>
 </file>
@@ -858,8 +858,8 @@
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -876,25 +876,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>160</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>161</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -902,19 +902,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -925,19 +925,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -948,19 +948,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G4" s="2">
         <v>1</v>
@@ -971,19 +971,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
@@ -994,19 +994,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
@@ -1017,19 +1017,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -1040,19 +1040,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
@@ -1063,16 +1063,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -1083,19 +1083,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
@@ -1106,16 +1106,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -1126,19 +1126,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G12" s="2">
         <v>1</v>
@@ -1149,19 +1149,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G13" s="2">
         <v>1</v>
@@ -1172,19 +1172,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G14" s="2">
         <v>1</v>
@@ -1195,19 +1195,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
@@ -1218,19 +1218,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G16" s="2">
         <v>1</v>
@@ -1241,16 +1241,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G17" s="2">
         <v>0</v>
@@ -1261,19 +1261,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G18" s="2">
         <v>1</v>
@@ -1284,16 +1284,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
@@ -1304,16 +1304,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G20" s="2">
         <v>0</v>
@@ -1324,19 +1324,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G21" s="2">
         <v>1</v>
@@ -1347,19 +1347,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G22" s="2">
         <v>1</v>
@@ -1370,19 +1370,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G23" s="2">
         <v>1</v>
@@ -1393,19 +1393,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G24" s="2">
         <v>1</v>
@@ -1416,19 +1416,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G25" s="2">
         <v>1</v>
@@ -1439,19 +1439,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G26" s="2">
         <v>1</v>
@@ -1462,19 +1462,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G27" s="2">
         <v>1</v>
@@ -1485,19 +1485,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G28" s="2">
         <v>1</v>
@@ -1508,19 +1508,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G29" s="2">
         <v>1</v>
@@ -1531,19 +1531,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G30" s="2">
         <v>1</v>
@@ -1554,19 +1554,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G31" s="2">
         <v>1</v>
@@ -1577,19 +1577,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G32" s="2">
         <v>1</v>
@@ -1600,19 +1600,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G33" s="2">
         <v>1</v>
@@ -1623,16 +1623,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G34" s="2">
         <v>0</v>
@@ -1643,19 +1643,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G35" s="2">
         <v>1</v>
@@ -1666,19 +1666,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G36" s="2">
         <v>1</v>
@@ -1689,19 +1689,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G37" s="2">
         <v>1</v>
@@ -1712,19 +1712,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G38" s="2">
         <v>1</v>
@@ -1735,19 +1735,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G39" s="2">
         <v>1</v>
@@ -1758,19 +1758,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G40" s="2">
         <v>1</v>
@@ -1781,19 +1781,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G41" s="2">
         <v>1</v>
@@ -1804,19 +1804,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G42" s="2">
         <v>1</v>
@@ -1827,19 +1827,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G43" s="2">
         <v>1</v>
@@ -1850,19 +1850,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G44" s="2">
         <v>1</v>
@@ -1873,19 +1873,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G45" s="2">
         <v>1</v>
@@ -1896,19 +1896,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G46" s="2">
         <v>1</v>
@@ -1919,19 +1919,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G47" s="2">
         <v>1</v>
@@ -1942,19 +1942,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G48" s="2">
         <v>0</v>
@@ -1965,19 +1965,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G49" s="2">
         <v>1</v>
@@ -1988,19 +1988,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G50" s="2">
         <v>1</v>
@@ -2011,19 +2011,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G51" s="2">
         <v>1</v>
@@ -2034,19 +2034,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G52" s="2">
         <v>1</v>
@@ -2057,19 +2057,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G53" s="2">
         <v>1</v>
@@ -2080,19 +2080,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G54" s="2">
         <v>1</v>
@@ -2103,19 +2103,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G55" s="2">
         <v>1</v>
@@ -2126,19 +2126,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G56" s="2">
         <v>0</v>
@@ -2149,19 +2149,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G57" s="2">
         <v>1</v>
@@ -2172,19 +2172,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G58" s="2">
         <v>1</v>
@@ -2195,19 +2195,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G59" s="2">
         <v>1</v>
@@ -2218,19 +2218,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G60" s="2">
         <v>1</v>
@@ -2241,19 +2241,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G61" s="2">
         <v>0</v>
@@ -2264,19 +2264,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G62" s="2">
         <v>0</v>
@@ -2287,19 +2287,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G63" s="2">
         <v>0</v>
@@ -2310,19 +2310,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G64" s="2">
         <v>0</v>
@@ -2333,19 +2333,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G65" s="2">
         <v>0</v>
@@ -2356,19 +2356,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G66" s="2">
         <v>0</v>
@@ -2379,19 +2379,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G67" s="2">
         <v>1</v>
@@ -2402,19 +2402,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G68" s="2">
         <v>1</v>
@@ -2425,19 +2425,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G69" s="2">
         <v>1</v>
@@ -2448,19 +2448,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G70" s="2">
         <v>1</v>
@@ -2471,19 +2471,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G71" s="2">
         <v>1</v>
@@ -2494,19 +2494,19 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G72" s="2">
         <v>1</v>
@@ -2517,19 +2517,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G73" s="2">
         <v>1</v>
@@ -2540,19 +2540,19 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G74" s="2">
         <v>1</v>
@@ -2563,19 +2563,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G75" s="2">
         <v>1</v>
@@ -2586,19 +2586,19 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G76" s="2">
         <v>1</v>
@@ -2609,19 +2609,19 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G77" s="2">
         <v>1</v>
@@ -2632,16 +2632,16 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G78" s="2">
         <v>0</v>
@@ -2652,16 +2652,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G79" s="2">
         <v>0</v>
@@ -2672,16 +2672,16 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G80" s="2">
         <v>0</v>
@@ -2692,16 +2692,16 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G81" s="2">
         <v>1</v>
@@ -2712,19 +2712,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G82" s="2">
         <v>0</v>
@@ -2735,19 +2735,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G83" s="2">
         <v>1</v>
@@ -2758,19 +2758,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G84" s="2">
         <v>1</v>
@@ -2781,19 +2781,19 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G85" s="2">
         <v>1</v>
@@ -2804,19 +2804,19 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G86" s="2">
         <v>0</v>
@@ -2827,19 +2827,19 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G87" s="2">
         <v>1</v>
@@ -2850,16 +2850,16 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G88" s="2">
         <v>0</v>
@@ -2870,19 +2870,19 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G89" s="2">
         <v>0</v>
@@ -2893,19 +2893,19 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G90" s="2">
         <v>1</v>
@@ -2916,16 +2916,16 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G91" s="2">
         <v>0</v>
@@ -2936,16 +2936,16 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G92" s="2">
         <v>0</v>
@@ -2956,16 +2956,16 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G93" s="2">
         <v>0</v>
@@ -2976,16 +2976,16 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G94" s="2">
         <v>0</v>
@@ -2996,16 +2996,16 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G95" s="2">
         <v>0</v>
@@ -3016,16 +3016,16 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G96" s="2">
         <v>0</v>
@@ -3036,16 +3036,16 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G97" s="2">
         <v>0</v>
@@ -3056,16 +3056,16 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G98" s="2">
         <v>0</v>
@@ -3076,16 +3076,16 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G99" s="2">
         <v>0</v>
@@ -3096,19 +3096,19 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G100" s="2">
         <v>1</v>
@@ -3119,16 +3119,16 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G101" s="2">
         <v>1</v>
@@ -3139,16 +3139,16 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G102" s="2">
         <v>0</v>
@@ -3159,16 +3159,16 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G103" s="2">
         <v>1</v>
@@ -3179,16 +3179,16 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G104" s="2">
         <v>0</v>
@@ -3199,16 +3199,16 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G105" s="2">
         <v>0</v>
@@ -3219,16 +3219,16 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G106" s="2">
         <v>0</v>
@@ -3239,16 +3239,16 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G107" s="2">
         <v>1</v>
@@ -3259,16 +3259,16 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G108" s="2">
         <v>0</v>
@@ -3279,16 +3279,16 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G109" s="2">
         <v>0</v>
@@ -3299,16 +3299,16 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G110" s="2">
         <v>0</v>
@@ -3319,16 +3319,16 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G111" s="2">
         <v>0</v>
@@ -3339,16 +3339,16 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G112" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
fitness function not completed yet
</commit_message>
<xml_diff>
--- a/DB/excersises DB.xlsx
+++ b/DB/excersises DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Git projects\AI-fitness-program-generator\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98590279-B5AD-494A-8799-2435871A27E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAFFA3F-AF6C-48FB-B330-AC563AD3705B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="527" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="168">
   <si>
     <t>Squat</t>
   </si>
@@ -450,9 +450,6 @@
     <t xml:space="preserve">Quadriceps, Inner Thighs, </t>
   </si>
   <si>
-    <t>Hamstrings, Core, Soulders, Forearms</t>
-  </si>
-  <si>
     <t>Back</t>
   </si>
   <si>
@@ -462,9 +459,6 @@
     <t>Traps, Biceps</t>
   </si>
   <si>
-    <t>Traps, Shoulders</t>
-  </si>
-  <si>
     <t>Traps, Core</t>
   </si>
   <si>
@@ -483,18 +477,6 @@
     <t>Chest</t>
   </si>
   <si>
-    <t>Triceps, Shoulders</t>
-  </si>
-  <si>
-    <t>Upper Chest</t>
-  </si>
-  <si>
-    <t>Lower Chest</t>
-  </si>
-  <si>
-    <t>Lats, Shoulders</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -514,6 +496,39 @@
   </si>
   <si>
     <t>isComplex</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Legs</t>
+  </si>
+  <si>
+    <t>Pectoralis</t>
+  </si>
+  <si>
+    <t>Upper Pectoralis</t>
+  </si>
+  <si>
+    <t>Lower Pectoralis</t>
+  </si>
+  <si>
+    <t>Deltoids</t>
+  </si>
+  <si>
+    <t>Triceps, Deltoids</t>
+  </si>
+  <si>
+    <t>Lats, Deltoids</t>
+  </si>
+  <si>
+    <t>Traps, Deltoids</t>
+  </si>
+  <si>
+    <t>Hamstrings, Core, Deltoids, Forearms</t>
+  </si>
+  <si>
+    <t>Arms</t>
   </si>
 </sst>
 </file>
@@ -855,72 +870,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="2"/>
+    <col min="3" max="3" width="9.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -928,22 +951,25 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -951,22 +977,25 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -974,22 +1003,25 @@
         <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -997,22 +1029,25 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1020,22 +1055,25 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1043,22 +1081,25 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1066,19 +1107,22 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1086,22 +1130,25 @@
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1109,19 +1156,22 @@
         <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1129,22 +1179,25 @@
         <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1152,22 +1205,25 @@
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1175,22 +1231,25 @@
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1198,22 +1257,25 @@
         <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1221,22 +1283,25 @@
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1244,19 +1309,22 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1264,22 +1332,25 @@
         <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1287,19 +1358,22 @@
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1307,19 +1381,22 @@
         <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1327,22 +1404,25 @@
         <v>29</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1350,22 +1430,25 @@
         <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="E22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1373,22 +1456,25 @@
         <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>1</v>
+        <v>141</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1396,22 +1482,25 @@
         <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1419,22 +1508,25 @@
         <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1442,22 +1534,25 @@
         <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1465,22 +1560,25 @@
         <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1488,22 +1586,25 @@
         <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1511,22 +1612,25 @@
         <v>36</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>145</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1534,22 +1638,25 @@
         <v>37</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1557,22 +1664,25 @@
         <v>45</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1580,22 +1690,25 @@
         <v>46</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1603,22 +1716,25 @@
         <v>47</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1626,19 +1742,22 @@
         <v>48</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1646,22 +1765,25 @@
         <v>49</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E35" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1669,22 +1791,25 @@
         <v>50</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1692,22 +1817,25 @@
         <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1715,22 +1843,25 @@
         <v>53</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1738,22 +1869,25 @@
         <v>54</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1761,22 +1895,25 @@
         <v>56</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1784,22 +1921,25 @@
         <v>57</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1807,22 +1947,25 @@
         <v>58</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1830,22 +1973,25 @@
         <v>59</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1853,22 +1999,25 @@
         <v>60</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G44" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1876,22 +2025,25 @@
         <v>61</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G45" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1899,22 +2051,25 @@
         <v>62</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E46" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1922,22 +2077,25 @@
         <v>63</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E47" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1945,22 +2103,25 @@
         <v>64</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G48" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1968,22 +2129,25 @@
         <v>65</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1991,22 +2155,25 @@
         <v>66</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2014,22 +2181,25 @@
         <v>67</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2037,22 +2207,25 @@
         <v>68</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2060,22 +2233,25 @@
         <v>69</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E53" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G53" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2083,22 +2259,25 @@
         <v>70</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E54" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2106,22 +2285,25 @@
         <v>71</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G55" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2129,22 +2311,25 @@
         <v>72</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="E56" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G56" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2152,22 +2337,25 @@
         <v>73</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2175,22 +2363,25 @@
         <v>74</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="E58" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2198,22 +2389,25 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E59" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G59" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2221,22 +2415,25 @@
         <v>76</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E60" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G60" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2244,22 +2441,25 @@
         <v>77</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="E61" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G61" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2267,22 +2467,25 @@
         <v>78</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G62" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2290,22 +2493,25 @@
         <v>79</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="E63" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G63" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2313,22 +2519,25 @@
         <v>80</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="E64" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F64" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G64" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H64" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2336,22 +2545,25 @@
         <v>81</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>91</v>
+        <v>160</v>
       </c>
       <c r="E65" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G65" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2359,22 +2571,25 @@
         <v>82</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="E66" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G66" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H66" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2382,22 +2597,25 @@
         <v>83</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D67" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2405,22 +2623,25 @@
         <v>84</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D68" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F68" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -2428,22 +2649,25 @@
         <v>85</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="E69" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G69" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -2451,22 +2675,25 @@
         <v>87</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E70" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G70" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -2474,22 +2701,25 @@
         <v>88</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E71" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -2500,19 +2730,22 @@
         <v>91</v>
       </c>
       <c r="D72" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F72" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G72" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -2523,19 +2756,22 @@
         <v>91</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -2546,19 +2782,22 @@
         <v>91</v>
       </c>
       <c r="D74" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G74" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H74" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -2569,19 +2808,22 @@
         <v>91</v>
       </c>
       <c r="D75" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F75" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G75" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H75" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -2592,19 +2834,22 @@
         <v>91</v>
       </c>
       <c r="D76" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G76" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H76" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -2615,19 +2860,22 @@
         <v>91</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G77" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G77" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -2637,17 +2885,20 @@
       <c r="C78" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="D78" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F78" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G78" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H78" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -2657,17 +2908,20 @@
       <c r="C79" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="D79" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F79" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G79" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H79" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -2677,17 +2931,20 @@
       <c r="C80" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="D80" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F80" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G80" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H80" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -2697,17 +2954,20 @@
       <c r="C81" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>1</v>
+      <c r="D81" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G81" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H81" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2718,19 +2978,22 @@
         <v>91</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>1</v>
+        <v>142</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G82" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H82" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2741,19 +3004,22 @@
         <v>91</v>
       </c>
       <c r="D83" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F83" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G83" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H83" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -2764,19 +3030,22 @@
         <v>91</v>
       </c>
       <c r="D84" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F84" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G84" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G84" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H84" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -2787,19 +3056,22 @@
         <v>91</v>
       </c>
       <c r="D85" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F85" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G85" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H85" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -2810,19 +3082,22 @@
         <v>91</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="E86" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F86" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G86" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H86" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -2833,19 +3108,22 @@
         <v>91</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="E87" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F87" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G87" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H87" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -2855,17 +3133,20 @@
       <c r="C88" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="D88" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F88" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G88" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H88" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -2876,19 +3157,22 @@
         <v>91</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="E89" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G89" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G89" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -2899,19 +3183,22 @@
         <v>91</v>
       </c>
       <c r="D90" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G90" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G90" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H90" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -2919,19 +3206,22 @@
         <v>111</v>
       </c>
       <c r="C91" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F91" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G91" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H91" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -2939,19 +3229,22 @@
         <v>113</v>
       </c>
       <c r="C92" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E92" s="2" t="s">
+      <c r="F92" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F92" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G92" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G92" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -2959,19 +3252,22 @@
         <v>114</v>
       </c>
       <c r="C93" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F93" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G93" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G93" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H93" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -2979,19 +3275,22 @@
         <v>115</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F94" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G94" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H94" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -2999,19 +3298,22 @@
         <v>116</v>
       </c>
       <c r="C95" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="F95" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F95" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G95" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H95" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -3019,19 +3321,22 @@
         <v>118</v>
       </c>
       <c r="C96" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="F96" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F96" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G96" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H96" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -3039,19 +3344,22 @@
         <v>119</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="F97" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F97" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G97" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G97" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H97" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -3059,19 +3367,22 @@
         <v>121</v>
       </c>
       <c r="C98" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D98" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F98" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G98" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H98" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -3079,19 +3390,22 @@
         <v>122</v>
       </c>
       <c r="C99" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F99" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G99" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H99" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -3099,22 +3413,25 @@
         <v>123</v>
       </c>
       <c r="C100" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="E100" s="2" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G100" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H100" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -3122,19 +3439,22 @@
         <v>125</v>
       </c>
       <c r="C101" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F101" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G101" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H101" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -3142,19 +3462,22 @@
         <v>126</v>
       </c>
       <c r="C102" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D102" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F102" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G102" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H102" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -3162,19 +3485,22 @@
         <v>127</v>
       </c>
       <c r="C103" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D103" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F103" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G103" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H103" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -3182,19 +3508,22 @@
         <v>128</v>
       </c>
       <c r="C104" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E104" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F104" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G104" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H104" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -3202,19 +3531,22 @@
         <v>129</v>
       </c>
       <c r="C105" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D105" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E105" s="2" t="s">
+      <c r="F105" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F105" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G105" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H105" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -3222,19 +3554,22 @@
         <v>130</v>
       </c>
       <c r="C106" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D106" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E106" s="2" t="s">
+      <c r="F106" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F106" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G106" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H106" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -3242,19 +3577,22 @@
         <v>131</v>
       </c>
       <c r="C107" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E107" s="2" t="s">
+      <c r="F107" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F107" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G107" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H107" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -3262,19 +3600,22 @@
         <v>132</v>
       </c>
       <c r="C108" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D108" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E108" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F108" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G108" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H108" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -3282,19 +3623,22 @@
         <v>133</v>
       </c>
       <c r="C109" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D109" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E109" s="2" t="s">
+      <c r="F109" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F109" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G109" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H109" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -3302,19 +3646,22 @@
         <v>134</v>
       </c>
       <c r="C110" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E110" s="2" t="s">
+      <c r="F110" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F110" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G110" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H110" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -3322,19 +3669,22 @@
         <v>135</v>
       </c>
       <c r="C111" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D111" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="F111" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F111" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G111" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G111" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H111" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -3342,15 +3692,18 @@
         <v>136</v>
       </c>
       <c r="C112" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D112" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="F112" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F112" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G112" s="2">
+      <c r="G112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H112" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
genetic algorithm fllow finished
</commit_message>
<xml_diff>
--- a/DB/excersises DB.xlsx
+++ b/DB/excersises DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Git projects\AI-fitness-program-generator\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAFFA3F-AF6C-48FB-B330-AC563AD3705B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EB46E9-E1CC-4E3C-9DA9-B9F5F41E24B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="527" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="169">
   <si>
     <t>Squat</t>
   </si>
@@ -529,6 +529,9 @@
   </si>
   <si>
     <t>Arms</t>
+  </si>
+  <si>
+    <t>Rear Deltoids</t>
   </si>
 </sst>
 </file>
@@ -873,8 +876,8 @@
   <dimension ref="A1:I112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L103" sqref="L103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2932,7 +2935,7 @@
         <v>91</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>4</v>
@@ -3082,7 +3085,7 @@
         <v>91</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>142</v>
@@ -3108,7 +3111,7 @@
         <v>91</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>142</v>
@@ -3134,7 +3137,7 @@
         <v>91</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>4</v>

</xml_diff>